<commit_message>
make python file for running
</commit_message>
<xml_diff>
--- a/news-crawl-result-test2.xlsx
+++ b/news-crawl-result-test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/master/dev/PythonPr/news-crawler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E39C7D-4EAF-8D42-87D6-3168E965F675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4D2B5A-E0E9-0940-A7D3-5A04C43F2683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="1260" windowWidth="30240" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="262">
   <si>
     <t>title</t>
   </si>
@@ -31,9 +31,6 @@
     <t>url</t>
   </si>
   <si>
-    <t>501st Military Intelligence Brigade strengthens alliance by hosting ROK/U.S. Intelligence Reception</t>
-  </si>
-  <si>
     <t>USAG HUMPHREYS, South Korea — Intelligence professionals from across the Republic of Korea and U.S. Army Intelligence and Security Command came together for a night to celebrate the alliance at the Morning Calm Center on Camp Humphreys, Feb. 2, 2023. The 2023 ROK/U.S. Intelligence Community Reception, hosted by the 501st Military Intelligence Brigade on behalf of INSCOM, provided an opportunity for U.S. Intelligence professionals to meet and develop rapport with key ROK national-level intelligence, security, and law enforcement officials who support the combined intelligence missions of United States Forces Korea, INSCOM, and the 501st MI Brigade. The night began with a social hour and food service, followed by the receiving line where the INSCOM and 501st MI Brigade command teams formally greeted guests. Attendees included senior leaders from across the Korean peninsula including Maj. Gen. Joseph D’costa, deputy commanding general, sustainment, Eighth Army; Brig. Gen. Richard Appelhans, J-2, USFK; Brig. Gen. Ju, Jung Woon, intelligence director in G-2/3, ROK Army headquarters; Maj. Gen. Son, Sug Rag, C-2, Combined Forces Command; Maj. Gen. Kim, Dong Ho, director of Doctrine Development, ROK Army Training Doctrine and Command; and Mr. Kim, Yong Ho, intelligence director, Korea Defense Intelligence Agency. Col. Lisa Winegar, commander, 501st MI Brigade, welcomed guests and remarked that maintaining friendship and strengthening the bond between the ROK and U.S. is the key to the two countries’ collective success. “Your attendance at our combined New Year’s celebration demonstrates the commitment we both share to an iron clad ROK/U.S. alliance,” Winegar said. “I am hopeful our continued collaboration and friendship will further strengthen the alliance. The hospitality of our ROK partners to their U.S. counterparts is unlike anything I have experienced anywhere else in my career.” Winegar continued, “Our combined training and operations are important, but the real secret to our strong ROK/U.S. alliance is through our deep and unwavering friendship. Whether sharing the love of Korean food through a monthly dinner or competing with one another through a friendly game of soccer, this friendship allows us to recognize our shared values and interests.” Maj. Gen. Michele Bredenkamp, INSCOM commanding general, also expressed her gratitude, remarking that the event is very special for her and the INSCOM members. “Tonight is an exciting night for many of us, especially for INSCOM. Due to the COVID-19 pandemic, we were unable to celebrate our intelligence partnership through an in-person annual reception since 2019,” Bredenkamp said. She noted how grateful she was to have the opportunity to attend in-person and begin the New Year with a great start after the long struggle of COVID-19. Bredenkamp went on to say that it takes the combined team to promote security and strengthen stability in the region and around the world. She then stated, “we must continue to foster the strength of our relationships, which takes time and effort to maintain and grow. We truly value our partnership and continue to invest in strengthening our alliance.” Bredenkamp, Winegar, and the two ROK guests of honor, Kim and Son, cut a ceremonial cake to end the formal portion of the reception. The reception featured Eighth Army Band musical performances throughout the event.</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
   </si>
   <si>
     <t>Craving Korean barbecue? You can get some at this new Northville Township restaurant</t>
-  </si>
-  <si>
-    <t>NORTHVILLE TWP. — It's been nothing but growth for Min Kyu Kim's fast-casual Korean Kimchi Box restaurants the last two years, and now he's bringing a new concept to his home community. Enter Kimchi Box Plus, an expanded offering which adds Korean barbecue to the menu. It's a concept, Kim said, that he hopes will introduce the cuisine to a new audience that may not have tried it. "I want to bring more approachable Korean barbecue," he said. "Normally, you would go and the menu is pretty complicated. You don't really know what to do." The restaurant at 18875 Traditions Drive, opened in early February in the former Tom &amp; Chee in the Northville Park Place shopping center near Seven Mile and Haggerty roads. Kim has taken the space and completely transformed it, adding tables complete with grills and vents. The location is the eighth Kimchi Box to open since it began in Sterling Heights in 2021. Today, there are locations in Plymouth Township, Novi, East Lansing and elsewhere. The Northville Township location is the lone Kimchi Box to offer Korean barbecue. "We did have a lot of anticipation because it's been under construction for a while now," Kim said. "This is the only one in Northville." Guests who come sit down and have a variety of options of food to choose from. The gas grill at the table is lit and guests can cook their food, including pork belly, brisket or kalbi, which is marinated boneless short ribs. The cooked food comes with a whole host of sides, including things like broccoli, kimchi and more. The traditional way to prepare the food is for guests to cook it themselves. Kim said some guests are unsure of how to do it, and sometimes staff can jump in to help them and show them the proper way. The restaurant also offers a full bar, including beer, wine, spirits and drinks from places like Korea and Japan. More:Banditos Restaurant &amp; Saloon brings Latin flavor to Milford More:Historic items discovered, saved in making of new South Lyon restaurant Dua Vino More:Historic Hines Park mills could begin seeing work this year The restaurant is open 11 a.m. to 10 p.m. daily. More information, including a menu, can be found at kimchiboxusa.com. The restaurant offers dine-in, carryout and delivery through some third-party apps. Kim, who moved to the United States from South Korea as a child, said his hope with his restaurants is to showcase South Korean food and bring a new flavor in a style not seen before, especially in Michigan. "I do research and what mostly exists is Korean fried chicken," he said of similar places. "I'm trying to put Korean fast casual on the map." Contact reporter David Veselenak at dveselenak@hometownlife.com or 734-678-6728. Follow him on Twitter @davidveselenak. Get the latest headlines for metro Detroit every morning in your mailbox by signing up for our daily briefings newsletter.</t>
   </si>
   <si>
     <t>https://news.google.com/articles/CBMilwFodHRwczovL3d3dy5ob21ldG93bmxpZmUuY29tL3N0b3J5L2xpZmUvZm9vZC8yMDIzLzAyLzI3L25ldy1raW1jaGktYm94LXBsdXMtcmVzdGF1cmFudC1pbi1ub3J0aHZpbGxlLXRvd25zaGlwLWNvb2tzLXNlcnZlcy1rb3JlYW4tYmFyYmVjdWUvNjk5NDAwODcwMDcv0gEA?hl=en-US&amp;gl=US&amp;ceid=US%3Aen</t>
@@ -1041,6 +1035,18 @@
   </si>
   <si>
     <t>https://news.google.com/articles/CBMiLWh0dHBzOi8vd3d3Lmh1bWFuaXRpZXMudWNpLmVkdS9uZXdzL3Nsb3ctYnVybtIBAA?hl=en-US&amp;gl=US&amp;ceid=US%3Aen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NORTHVILLE TWP. — It's been nothing but growth for Min Kyu Kim's fast-casual Korean Kimchi Box restaurants the last two years, and now he's bringing a new concept to his home community. Enter Kimchi Box Plus, an expanded offering which adds Korean barbecue to the menu. It's a concept, Kim said, that he hopes will introduce the cuisine to a new audience that may not have tried it. "I want to bring more approachable Korean barbecue," he said. "Normally, you would go and the menu is pretty complicated. You don't really know what to do." The restaurant at 18875 Traditions Drive, opened in early February in the former Tom &amp; Chee in the Northville Park Place shopping center near Seven Mile and Haggerty roads. Kim has taken the space and completely transformed it, adding tables complete with grills and vents. The location is the eighth Kimchi Box to open since it began in Sterling Heights in 2021. Today, there are locations in Plymouth Township, Novi, East Lansing and elsewhere. The Northville Township location is the lone Kimchi Box to offer Korean barbecue. "We did have a lot of anticipation because it's been under construction for a while now," Kim said. "This is the only one in Northville." Guests who come sit down and have a variety of options of food to choose from. The gas grill at the table is lit and guests can cook their food, including pork belly, brisket or kalbi, which is marinated boneless short ribs. The cooked food comes with a whole host of sides, including things like broccoli, kimchi and more. The traditional way to prepare the food is for guests to cook it themselves. Kim said some guests are unsure of how to do it, and sometimes staff can jump in to help them and show them the proper way. The restaurant also offers a full bar, including beer, wine, spirits and drinks from places like Korea and Japan. More:Banditos Restaurant &amp; Saloon brings Latin flavor to Milford More:Historic items discovered, saved in making of new South Lyon restaurant Dua Vino More:Historic Hines Park mills could begin seeing work this year The restaurant is open 11 a.m. to 10 p.m. daily. More information, including a menu, can be found at kimchiboxusa.com. The restaurant offers dine-in, carryout and delivery through some third-party apps. Kim, who moved to the United States from South Korea as a child, said his hope with his restaurants is to showcase South Korean food and bring a new flavor in a style not seen before, especially in Michigan. "I do research and what mostly exists is Korean fried chicken," he said of similar places. "I'm trying to put Korean fast casual on the map." Contact reporter David Veselenak at dveselenak@hometownlife.com or 734-678-6728. Follow him on Twitter @davidveselenak. Get the latest headlines for metro Detroit every morning in your mailbox by signing up for our daily briefings newsletter.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>501st Military Intelligence Brigade strengthens alliance by hosting ROK/U.S. Intelligence Reception</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://news.google.com/articles/CBMihQFodHRwczovL3d3dy5hcm15Lm1pbC9hcnRpY2xlLzI2NDI1NS81MDFzdF9taWxpdGFyeV9pbnRlbGxpZ2VuY2VfYnJpZ2FkZV9zdHJlbmd0aGVuc19hbGxpYW5jZV9ieV9ob3N0aW5nX3Jva3Vfc19pbnRlbGxpZ2VuY2VfcmVjZXB0aW9u0gEA?hl=en-US&amp;gl=US&amp;ceid=US%3Aen</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1437,13 +1443,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1462,13 +1469,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="D2" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1476,13 +1483,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1490,13 +1497,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1504,13 +1511,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1518,13 +1525,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1532,13 +1539,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1546,13 +1553,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1560,13 +1567,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1574,13 +1581,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1588,10 +1595,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1599,13 +1606,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1613,13 +1620,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1627,13 +1634,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1641,10 +1648,10 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1652,10 +1659,10 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1663,13 +1670,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
         <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1677,10 +1684,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1688,13 +1695,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
         <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1702,13 +1709,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
         <v>48</v>
-      </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1716,13 +1723,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
         <v>51</v>
-      </c>
-      <c r="C21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1730,13 +1737,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1744,13 +1751,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
         <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1758,13 +1765,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
         <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1772,13 +1779,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1786,13 +1793,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
         <v>63</v>
-      </c>
-      <c r="C26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1800,13 +1807,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1814,13 +1821,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
         <v>67</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1828,13 +1835,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s">
         <v>70</v>
-      </c>
-      <c r="C29" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1842,13 +1849,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
         <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1856,10 +1863,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1867,13 +1874,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" t="s">
         <v>78</v>
-      </c>
-      <c r="C32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1881,13 +1888,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" t="s">
         <v>81</v>
-      </c>
-      <c r="C33" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1895,13 +1902,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
         <v>84</v>
-      </c>
-      <c r="C34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1909,13 +1916,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" t="s">
         <v>87</v>
-      </c>
-      <c r="C35" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1923,13 +1930,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1937,13 +1944,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" t="s">
         <v>90</v>
-      </c>
-      <c r="C37" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1951,13 +1958,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
         <v>93</v>
-      </c>
-      <c r="C38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1965,13 +1972,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" t="s">
         <v>96</v>
-      </c>
-      <c r="C39" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1979,13 +1986,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
         <v>99</v>
-      </c>
-      <c r="C40" t="s">
-        <v>100</v>
-      </c>
-      <c r="D40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1993,10 +2000,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2004,13 +2011,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" t="s">
         <v>104</v>
-      </c>
-      <c r="C42" t="s">
-        <v>105</v>
-      </c>
-      <c r="D42" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2018,13 +2025,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" t="s">
         <v>107</v>
-      </c>
-      <c r="C43" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2032,13 +2039,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" t="s">
         <v>110</v>
-      </c>
-      <c r="C44" t="s">
-        <v>111</v>
-      </c>
-      <c r="D44" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2046,13 +2053,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2060,13 +2067,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2074,13 +2081,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2088,10 +2095,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D48" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2099,13 +2106,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" t="s">
         <v>118</v>
-      </c>
-      <c r="C49" t="s">
-        <v>119</v>
-      </c>
-      <c r="D49" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2113,13 +2120,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
         <v>121</v>
-      </c>
-      <c r="C50" t="s">
-        <v>122</v>
-      </c>
-      <c r="D50" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2127,13 +2134,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" t="s">
         <v>124</v>
-      </c>
-      <c r="C51" t="s">
-        <v>125</v>
-      </c>
-      <c r="D51" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2141,13 +2148,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D52" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2155,13 +2162,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" t="s">
         <v>129</v>
-      </c>
-      <c r="C53" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2169,13 +2176,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" t="s">
         <v>132</v>
-      </c>
-      <c r="C54" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2183,13 +2190,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" t="s">
         <v>135</v>
-      </c>
-      <c r="C55" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2197,13 +2204,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" t="s">
         <v>138</v>
-      </c>
-      <c r="C56" t="s">
-        <v>139</v>
-      </c>
-      <c r="D56" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2211,10 +2218,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2222,13 +2229,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2236,13 +2243,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" t="s">
+        <v>142</v>
+      </c>
+      <c r="D59" t="s">
         <v>143</v>
-      </c>
-      <c r="C59" t="s">
-        <v>144</v>
-      </c>
-      <c r="D59" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2250,13 +2257,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" t="s">
+        <v>145</v>
+      </c>
+      <c r="D60" t="s">
         <v>146</v>
-      </c>
-      <c r="C60" t="s">
-        <v>147</v>
-      </c>
-      <c r="D60" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2264,10 +2271,10 @@
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2275,13 +2282,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
+        <v>149</v>
+      </c>
+      <c r="C62" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" t="s">
         <v>151</v>
-      </c>
-      <c r="C62" t="s">
-        <v>152</v>
-      </c>
-      <c r="D62" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2289,13 +2296,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" t="s">
+        <v>153</v>
+      </c>
+      <c r="D63" t="s">
         <v>154</v>
-      </c>
-      <c r="C63" t="s">
-        <v>155</v>
-      </c>
-      <c r="D63" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2303,13 +2310,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" t="s">
+        <v>156</v>
+      </c>
+      <c r="D64" t="s">
         <v>157</v>
-      </c>
-      <c r="C64" t="s">
-        <v>158</v>
-      </c>
-      <c r="D64" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2317,13 +2324,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
+        <v>158</v>
+      </c>
+      <c r="C65" t="s">
+        <v>159</v>
+      </c>
+      <c r="D65" t="s">
         <v>160</v>
-      </c>
-      <c r="C65" t="s">
-        <v>161</v>
-      </c>
-      <c r="D65" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2331,13 +2338,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>161</v>
+      </c>
+      <c r="C66" t="s">
+        <v>162</v>
+      </c>
+      <c r="D66" t="s">
         <v>163</v>
-      </c>
-      <c r="C66" t="s">
-        <v>164</v>
-      </c>
-      <c r="D66" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2345,13 +2352,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67" t="s">
+        <v>165</v>
+      </c>
+      <c r="D67" t="s">
         <v>166</v>
-      </c>
-      <c r="C67" t="s">
-        <v>167</v>
-      </c>
-      <c r="D67" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2359,13 +2366,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
+        <v>167</v>
+      </c>
+      <c r="C68" t="s">
+        <v>168</v>
+      </c>
+      <c r="D68" t="s">
         <v>169</v>
-      </c>
-      <c r="C68" t="s">
-        <v>170</v>
-      </c>
-      <c r="D68" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2373,13 +2380,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2387,13 +2394,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
+        <v>170</v>
+      </c>
+      <c r="C70" t="s">
+        <v>171</v>
+      </c>
+      <c r="D70" t="s">
         <v>172</v>
-      </c>
-      <c r="C70" t="s">
-        <v>173</v>
-      </c>
-      <c r="D70" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2401,13 +2408,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C71" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D71" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2415,13 +2422,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
+        <v>175</v>
+      </c>
+      <c r="C72" t="s">
+        <v>176</v>
+      </c>
+      <c r="D72" t="s">
         <v>177</v>
-      </c>
-      <c r="C72" t="s">
-        <v>178</v>
-      </c>
-      <c r="D72" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2429,13 +2436,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
+        <v>178</v>
+      </c>
+      <c r="C73" t="s">
+        <v>179</v>
+      </c>
+      <c r="D73" t="s">
         <v>180</v>
-      </c>
-      <c r="C73" t="s">
-        <v>181</v>
-      </c>
-      <c r="D73" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2443,13 +2450,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" t="s">
+        <v>182</v>
+      </c>
+      <c r="D74" t="s">
         <v>183</v>
-      </c>
-      <c r="C74" t="s">
-        <v>184</v>
-      </c>
-      <c r="D74" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2457,13 +2464,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
+        <v>184</v>
+      </c>
+      <c r="C75" t="s">
+        <v>185</v>
+      </c>
+      <c r="D75" t="s">
         <v>186</v>
-      </c>
-      <c r="C75" t="s">
-        <v>187</v>
-      </c>
-      <c r="D75" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2471,13 +2478,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
+        <v>187</v>
+      </c>
+      <c r="C76" t="s">
+        <v>188</v>
+      </c>
+      <c r="D76" t="s">
         <v>189</v>
-      </c>
-      <c r="C76" t="s">
-        <v>190</v>
-      </c>
-      <c r="D76" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2485,13 +2492,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
+        <v>190</v>
+      </c>
+      <c r="C77" t="s">
+        <v>191</v>
+      </c>
+      <c r="D77" t="s">
         <v>192</v>
-      </c>
-      <c r="C77" t="s">
-        <v>193</v>
-      </c>
-      <c r="D77" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2499,13 +2506,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2513,13 +2520,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
+        <v>194</v>
+      </c>
+      <c r="C79" t="s">
+        <v>195</v>
+      </c>
+      <c r="D79" t="s">
         <v>196</v>
-      </c>
-      <c r="C79" t="s">
-        <v>197</v>
-      </c>
-      <c r="D79" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2527,13 +2534,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D80" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2541,13 +2548,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2555,13 +2562,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
+        <v>198</v>
+      </c>
+      <c r="C82" t="s">
+        <v>199</v>
+      </c>
+      <c r="D82" t="s">
         <v>200</v>
-      </c>
-      <c r="C82" t="s">
-        <v>201</v>
-      </c>
-      <c r="D82" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2569,13 +2576,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2583,13 +2590,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
+        <v>202</v>
+      </c>
+      <c r="C84" t="s">
+        <v>203</v>
+      </c>
+      <c r="D84" t="s">
         <v>204</v>
-      </c>
-      <c r="C84" t="s">
-        <v>205</v>
-      </c>
-      <c r="D84" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2597,13 +2604,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2611,13 +2618,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
+        <v>206</v>
+      </c>
+      <c r="C86" t="s">
+        <v>207</v>
+      </c>
+      <c r="D86" t="s">
         <v>208</v>
-      </c>
-      <c r="C86" t="s">
-        <v>209</v>
-      </c>
-      <c r="D86" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2625,13 +2632,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
+        <v>209</v>
+      </c>
+      <c r="C87" t="s">
+        <v>210</v>
+      </c>
+      <c r="D87" t="s">
         <v>211</v>
-      </c>
-      <c r="C87" t="s">
-        <v>212</v>
-      </c>
-      <c r="D87" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2639,13 +2646,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" t="s">
+        <v>213</v>
+      </c>
+      <c r="D88" t="s">
         <v>214</v>
-      </c>
-      <c r="C88" t="s">
-        <v>215</v>
-      </c>
-      <c r="D88" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2653,13 +2660,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
+        <v>215</v>
+      </c>
+      <c r="C89" t="s">
+        <v>216</v>
+      </c>
+      <c r="D89" t="s">
         <v>217</v>
-      </c>
-      <c r="C89" t="s">
-        <v>218</v>
-      </c>
-      <c r="D89" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2667,13 +2674,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
+        <v>218</v>
+      </c>
+      <c r="C90" t="s">
+        <v>219</v>
+      </c>
+      <c r="D90" t="s">
         <v>220</v>
-      </c>
-      <c r="C90" t="s">
-        <v>221</v>
-      </c>
-      <c r="D90" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2681,13 +2688,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2695,13 +2702,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
+        <v>221</v>
+      </c>
+      <c r="C92" t="s">
+        <v>222</v>
+      </c>
+      <c r="D92" t="s">
         <v>223</v>
-      </c>
-      <c r="C92" t="s">
-        <v>224</v>
-      </c>
-      <c r="D92" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2709,10 +2716,10 @@
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D93" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2720,13 +2727,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
+        <v>226</v>
+      </c>
+      <c r="C94" t="s">
+        <v>227</v>
+      </c>
+      <c r="D94" t="s">
         <v>228</v>
-      </c>
-      <c r="C94" t="s">
-        <v>229</v>
-      </c>
-      <c r="D94" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2734,13 +2741,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
+        <v>229</v>
+      </c>
+      <c r="C95" t="s">
+        <v>230</v>
+      </c>
+      <c r="D95" t="s">
         <v>231</v>
-      </c>
-      <c r="C95" t="s">
-        <v>232</v>
-      </c>
-      <c r="D95" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2748,13 +2755,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
+        <v>232</v>
+      </c>
+      <c r="C96" t="s">
+        <v>233</v>
+      </c>
+      <c r="D96" t="s">
         <v>234</v>
-      </c>
-      <c r="C96" t="s">
-        <v>235</v>
-      </c>
-      <c r="D96" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2762,13 +2769,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
+        <v>235</v>
+      </c>
+      <c r="C97" t="s">
+        <v>236</v>
+      </c>
+      <c r="D97" t="s">
         <v>237</v>
-      </c>
-      <c r="C97" t="s">
-        <v>238</v>
-      </c>
-      <c r="D97" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2776,13 +2783,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
+        <v>238</v>
+      </c>
+      <c r="C98" t="s">
+        <v>239</v>
+      </c>
+      <c r="D98" t="s">
         <v>240</v>
-      </c>
-      <c r="C98" t="s">
-        <v>241</v>
-      </c>
-      <c r="D98" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2790,13 +2797,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
+        <v>241</v>
+      </c>
+      <c r="C99" t="s">
+        <v>242</v>
+      </c>
+      <c r="D99" t="s">
         <v>243</v>
-      </c>
-      <c r="C99" t="s">
-        <v>244</v>
-      </c>
-      <c r="D99" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2804,13 +2811,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
+        <v>244</v>
+      </c>
+      <c r="C100" t="s">
+        <v>245</v>
+      </c>
+      <c r="D100" t="s">
         <v>246</v>
-      </c>
-      <c r="C100" t="s">
-        <v>247</v>
-      </c>
-      <c r="D100" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2818,7 +2825,7 @@
         <v>99</v>
       </c>
       <c r="D101" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2826,13 +2833,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2840,13 +2847,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D103" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2854,13 +2861,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
+        <v>249</v>
+      </c>
+      <c r="C104" t="s">
+        <v>250</v>
+      </c>
+      <c r="D104" t="s">
         <v>251</v>
-      </c>
-      <c r="C104" t="s">
-        <v>252</v>
-      </c>
-      <c r="D104" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2868,13 +2875,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
+        <v>252</v>
+      </c>
+      <c r="C105" t="s">
+        <v>253</v>
+      </c>
+      <c r="D105" t="s">
         <v>254</v>
-      </c>
-      <c r="C105" t="s">
-        <v>255</v>
-      </c>
-      <c r="D105" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2882,13 +2889,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
+        <v>255</v>
+      </c>
+      <c r="C106" t="s">
+        <v>256</v>
+      </c>
+      <c r="D106" t="s">
         <v>257</v>
-      </c>
-      <c r="C106" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" t="s">
-        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2900,6 +2907,7 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D46" r:id="rId1" xr:uid="{D8686B29-5E20-874F-A0A4-8F5A714FD5E9}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{A38741D1-A794-3B42-9CF3-D2795847EAF8}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>